<commit_message>
Added: Domain Model Support for Test Runner.
</commit_message>
<xml_diff>
--- a/DNS Response.xlsx
+++ b/DNS Response.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Texnomic.SecureDNS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AFEDF5F-34F3-4427-9620-D32F0C6F5673}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD8FD5A-1439-4641-A712-FA525616D453}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72456694-AFC5-4030-ADFB-E810E9A44ECB}"/>
+    <workbookView xWindow="-9885" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{72456694-AFC5-4030-ADFB-E810E9A44ECB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>00000000 00101110</t>
   </si>
@@ -49,9 +48,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Usigned 16-Bit Integer</t>
-  </si>
-  <si>
     <t>10011001 10000010</t>
   </si>
   <si>
@@ -68,9 +64,6 @@
   </si>
   <si>
     <t>0000</t>
-  </si>
-  <si>
-    <t>4 Bit Int</t>
   </si>
   <si>
     <t>Operation Code</t>
@@ -145,18 +138,9 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Facebook</t>
-  </si>
-  <si>
     <t>000011</t>
   </si>
   <si>
-    <t>01100011 01101111 01101101</t>
-  </si>
-  <si>
-    <t>Com</t>
-  </si>
-  <si>
     <t xml:space="preserve">00000000 </t>
   </si>
   <si>
@@ -178,15 +162,9 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>000000 00001100</t>
-  </si>
-  <si>
     <t>Lable Pointer</t>
   </si>
   <si>
-    <t>00000000 00000000 00000000 00010111</t>
-  </si>
-  <si>
     <t>TTL</t>
   </si>
   <si>
@@ -196,9 +174,6 @@
     <t>Record Length</t>
   </si>
   <si>
-    <t>10110011 00111100 11000000 00100100</t>
-  </si>
-  <si>
     <t>IP Address</t>
   </si>
   <si>
@@ -209,6 +184,63 @@
   </si>
   <si>
     <t>Compressed</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>2 Bit Flag</t>
+  </si>
+  <si>
+    <t>Unsigned 16-Bit Integer</t>
+  </si>
+  <si>
+    <t>Unsigned 6-Bit Integer</t>
+  </si>
+  <si>
+    <t>Unsigned 4-Bit Integer</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>No Error</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>179.60.192.36</t>
+  </si>
+  <si>
+    <t>Byte Per Character</t>
+  </si>
+  <si>
+    <t>01100011 01101111
+01101101</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Unsigned 14-Bit Integer</t>
+  </si>
+  <si>
+    <t>Unsigned 32-Bit Integer</t>
+  </si>
+  <si>
+    <t>00000000 00000000
+00000000 00010111</t>
+  </si>
+  <si>
+    <t>10110011 00111100
+11000000 00100100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    000000 00001100</t>
   </si>
 </sst>
 </file>
@@ -265,7 +297,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -276,6 +328,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F26A05FF-066E-4957-9102-4B75F480E473}" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:D31" xr:uid="{3CD634FE-8A16-4436-9222-961EE75A06A8}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CF807987-A851-4D74-8C6B-5666FC949DC1}" name="Binary" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2E682A01-1F24-488E-9AF8-1FA4CF503A32}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{6815714A-6D45-4AA0-8E7A-9BCA410D13E4}" name="Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F0D026F4-275B-4741-8C88-E53F97094D1F}" name="Value" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -575,18 +640,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450721F4-B21D-44A9-9BFF-EFC9D66297F6}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,21 +673,27 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>39298</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,312 +701,398 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>26</v>
+      <c r="D15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
+      <c r="D17" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D19" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D28" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>24</v>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>55</v>
+      <c r="D29" s="1">
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99824F88-7DB7-49DB-96EA-FD455F4D6ACF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>